<commit_message>
update views and templates
</commit_message>
<xml_diff>
--- a/PMS/resources/xlxsss/elective_priority_cleaned (1).xlsx
+++ b/PMS/resources/xlxsss/elective_priority_cleaned (1).xlsx
@@ -726,12 +726,16 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -999,1101 +1003,1102 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="61.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="74.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="71.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="58.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="61.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="74.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="0" t="s">
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="E22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="E24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="0" t="s">
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="0" t="s">
+      <c r="G28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="0" t="s">
+      <c r="F29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="H29" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="G30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="H30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="0" t="s">
+      <c r="F31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="H31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G32" s="0" t="s">
+      <c r="F32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="H32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="E33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="H33" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H34" s="0" t="s">
+      <c r="G34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="D36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="G36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H36" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="E37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="G37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="D38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="H38" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="G39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="H39" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" s="0" t="s">
+      <c r="G40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="G41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H41" s="0" t="s">
+      <c r="H41" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="G42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="H42" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="G43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="0" t="s">
+      <c r="H43" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G44" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H44" s="0" t="s">
+      <c r="G44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="G45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="H45" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="H46" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="D47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G47" s="0" t="s">
+      <c r="G47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="H47" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="G48" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="H48" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="E49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="G49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H49" s="0" t="s">
+      <c r="H49" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>